<commit_message>
fixed child weighted count issue in frequencies
</commit_message>
<xml_diff>
--- a/output/frequencies/VNM_children_2011.xlsx
+++ b/output/frequencies/VNM_children_2011.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="excl_bf_weighted" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="cont_1223_bf_weighted" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="mmf_ch_weighted" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -825,4 +827,820 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>cont_1223_bf</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Weighted_Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>46.1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>758.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>CH Sex: Female</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>45.4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>368.3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>CH Sex: Male</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>390.7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>48.3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>526.7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Urban</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>41</v>
+      </c>
+      <c r="C6" t="n">
+        <v>232.2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Central Highlands</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>61.7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>54.1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Mekong River Delta</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>113.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>North Central and Central Coast</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>53</v>
+      </c>
+      <c r="C9" t="n">
+        <v>160.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Northern Midlands and Mountain</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>57.3</v>
+      </c>
+      <c r="C10" t="n">
+        <v>153.6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Red River Delta</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>44.9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>156.3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Southeast</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>120.9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Mother Edu: Higher</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Mother Edu: None/ECE</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>54.2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>33.4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Mother Edu: Primary</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>45.4</v>
+      </c>
+      <c r="C15" t="n">
+        <v>113.4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Mother Edu: Secondary</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>48.2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>514.2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>47</v>
+      </c>
+      <c r="C17" t="n">
+        <v>144.3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Poor</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>49.8</v>
+      </c>
+      <c r="C18" t="n">
+        <v>130.7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Poorest</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="C19" t="n">
+        <v>165.4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Rich</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>144.7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Richest</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>34.8</v>
+      </c>
+      <c r="C21" t="n">
+        <v>173.7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Khmer</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="C22" t="n">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Kinh and Hoa</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>43</v>
+      </c>
+      <c r="C23" t="n">
+        <v>645.6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Mong</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>62.3</v>
+      </c>
+      <c r="C24" t="n">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Other/Missing</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>76.3</v>
+      </c>
+      <c r="C25" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Tay, Thai, Muong, Nung</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="C26" t="n">
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Elderly HoH: NO</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>46.1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>613.7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Elderly HoH: YES</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="C28" t="n">
+        <v>145.2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>42</v>
+      </c>
+      <c r="C29" t="n">
+        <v>185.4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="C30" t="n">
+        <v>573.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mmf_ch</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Weighted_Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>54.6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1099.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>CH Sex: Female</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>CH Sex: Male</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>57.6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>538.9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>54.4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Urban</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>54.9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>324.9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Central Highlands</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>75.59999999999999</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Mekong River Delta</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>183.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>North Central and Central Coast</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>224.1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Northern Midlands and Mountain</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>48.2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>218.8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Red River Delta</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>67.7</v>
+      </c>
+      <c r="C11" t="n">
+        <v>221.4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Southeast</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>61.8</v>
+      </c>
+      <c r="C12" t="n">
+        <v>176.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Mother Edu: Higher</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>60.2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>130.3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Mother Edu: None/ECE</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>42.1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Mother Edu: Primary</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="C15" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Mother Edu: Secondary</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>55</v>
+      </c>
+      <c r="C16" t="n">
+        <v>749.3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="C17" t="n">
+        <v>199.2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Poor</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>210.4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Poorest</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>234.2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Rich</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>56.9</v>
+      </c>
+      <c r="C20" t="n">
+        <v>212.3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Richest</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="C21" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Khmer</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="C22" t="n">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Kinh and Hoa</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>56</v>
+      </c>
+      <c r="C23" t="n">
+        <v>929.1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Mong</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="C24" t="n">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Other/Missing</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="C25" t="n">
+        <v>38.2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Tay, Thai, Muong, Nung</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>60.2</v>
+      </c>
+      <c r="C26" t="n">
+        <v>94.2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Elderly HoH: NO</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="C27" t="n">
+        <v>875.8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Elderly HoH: YES</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="C28" t="n">
+        <v>224.1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>64.90000000000001</v>
+      </c>
+      <c r="C29" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>849.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>